<commit_message>
[Feat] 낚시 NPC 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/Additional/Excel/FishingGuide.xlsx
+++ b/Assets/Resources/Additional/Excel/FishingGuide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\Become_Celebrity_on_Farm\Assets\Resources\Additional\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C45CE4C-2787-44F2-BB82-E783F83CE8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC95B1BA-E7E4-46DD-812F-8078C9F6DD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
-  <si>
-    <t>BlackSmith_0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
   <si>
     <t>Daily</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -33,31 +30,102 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Shop/OFF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>None</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>오늘도 왔는가</t>
-  </si>
-  <si>
-    <t>BlackSmith_0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>요즘 농사는 괜찮게 되고 있지?</t>
-  </si>
-  <si>
-    <t>좋은 상품이 들어왔는데 보고 가겠나?</t>
-  </si>
-  <si>
-    <t>우리 마을의 유일 마트라고</t>
-  </si>
-  <si>
-    <t>BlackSmith_3</t>
+    <t>저기 저 멀리 있는 선박 보여?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그런 낚시대로 뭘 낚을 수 있겠냐?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번에 새로온 주민이 너구나?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>왜 인어 처음봐?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MermaidSample</t>
+  </si>
+  <si>
+    <t>오늘 또 왔네?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아~ 신경 쓰지마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>니가 뭘 낚든 내 친구는 아니야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚시대가 그래서는 대어를 낚겠어?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나중에 다시오면 전문가 좀 불러줄까?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐야 그게 낚시대야?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚시 말고 뭐하고 살아?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>난 육지 이야기 듣는게 좋아</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OFF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그 주위에 신기한 물고기가 산다고 하더라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어부들이 어제 술 마시면서 말하던데</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나도 본적 없는데</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가끔 가다가 걷고 싶은거 있지?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사실 걸어본적도 없는데</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>너희도 수영하고 싶은거랑 비슷할 수도</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 더 좋은 낚시대를 얻고 싶다고?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>글쎄 아직 사람이 쓸 정도로 만들어지지 않았다고 하더라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무슨 이야기냐고?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인어가 쓰는 낚시대가 있는데 사람은 못쓴데</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -381,15 +449,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.625" customWidth="1"/>
+    <col min="1" max="1" width="53.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -397,75 +465,75 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>100</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="G1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -473,41 +541,497 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
         <v>100</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>